<commit_message>
Tests on different scenarios: - target and trajectory data missing - only target data missing
Signed-off-by: Cas Jiskoot <cas.jiskoot@ortec-finance.com>
</commit_message>
<xml_diff>
--- a/test/inputs/test_data_company.xlsx
+++ b/test/inputs/test_data_company.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\test\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casj\PycharmProjects\ITR\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAC0AB0-68AB-4808-AF5B-BD21E051D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,20 @@
     <sheet name="projected_target" sheetId="6" r:id="rId3"/>
     <sheet name="projected_ei_in_Wh" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -371,7 +382,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -464,29 +475,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R56" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:R56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R56" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:R56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="company_name"/>
-    <tableColumn id="2" name="company_id"/>
-    <tableColumn id="3" name="isic"/>
-    <tableColumn id="4" name="country"/>
-    <tableColumn id="20" name="region"/>
-    <tableColumn id="5" name="industry_level_1"/>
-    <tableColumn id="22" name="industry_level_2"/>
-    <tableColumn id="21" name="industry_level_3"/>
-    <tableColumn id="7" name="industry_level_4"/>
-    <tableColumn id="6" name="sector"/>
-    <tableColumn id="18" name="ghg_s1s2"/>
-    <tableColumn id="8" name="ghg_s3"/>
-    <tableColumn id="9" name="company_revenue"/>
-    <tableColumn id="10" name="company_market_cap"/>
-    <tableColumn id="11" name="company_enterprise_value"/>
-    <tableColumn id="12" name="company_total_assets" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="isic"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="country"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="region"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="industry_level_1"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="industry_level_2"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="industry_level_3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="industry_level_4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="sector"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ghg_s1s2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ghg_s3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="company_revenue"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="company_market_cap"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="company_enterprise_value"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="company_total_assets" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[company_market_cap]]*Q2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="company_cash_equivalents"/>
-    <tableColumn id="17" name="target_probability"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="company_cash_equivalents"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="target_probability"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -754,7 +765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2121,10 +2132,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -9409,11 +9420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15045,108 +15056,6 @@
       <c r="B56" t="s">
         <v>93</v>
       </c>
-      <c r="K56">
-        <v>0.64100565373528196</v>
-      </c>
-      <c r="L56">
-        <v>0.63266100451370499</v>
-      </c>
-      <c r="M56">
-        <v>0.65549322936238597</v>
-      </c>
-      <c r="N56">
-        <v>0.66206039012700302</v>
-      </c>
-      <c r="O56">
-        <v>0.64550888037382792</v>
-      </c>
-      <c r="P56">
-        <v>0.62895737062065282</v>
-      </c>
-      <c r="Q56">
-        <v>0.61240586086747772</v>
-      </c>
-      <c r="R56">
-        <v>0.59585435111430263</v>
-      </c>
-      <c r="S56">
-        <v>0.57930284136112753</v>
-      </c>
-      <c r="T56">
-        <v>0.56275133160795243</v>
-      </c>
-      <c r="U56">
-        <v>0.54619982185477733</v>
-      </c>
-      <c r="V56">
-        <v>0.52964831210160235</v>
-      </c>
-      <c r="W56">
-        <v>0.51309680234842725</v>
-      </c>
-      <c r="X56">
-        <v>0.4965452925952521</v>
-      </c>
-      <c r="Y56">
-        <v>0.479993782842077</v>
-      </c>
-      <c r="Z56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AA56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AB56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AC56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AD56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AE56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AF56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AG56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AH56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AI56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AJ56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AK56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AL56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AM56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AN56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AO56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AP56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AQ56">
-        <v>0.46344227308890196</v>
-      </c>
-      <c r="AR56">
-        <v>0.46344227308890196</v>
-      </c>
     </row>
     <row r="57" spans="1:44">
       <c r="A57" t="s">
@@ -15154,108 +15063,6 @@
       </c>
       <c r="B57" t="s">
         <v>94</v>
-      </c>
-      <c r="K57">
-        <v>7.8996951321949296E-2</v>
-      </c>
-      <c r="L57">
-        <v>7.7112657879593705E-2</v>
-      </c>
-      <c r="M57">
-        <v>8.0243540265543895E-2</v>
-      </c>
-      <c r="N57">
-        <v>8.1047472641410601E-2</v>
-      </c>
-      <c r="O57">
-        <v>7.9021285825375334E-2</v>
-      </c>
-      <c r="P57">
-        <v>7.6995099009340068E-2</v>
-      </c>
-      <c r="Q57">
-        <v>7.4968912193304801E-2</v>
-      </c>
-      <c r="R57">
-        <v>7.2942725377269535E-2</v>
-      </c>
-      <c r="S57">
-        <v>7.0916538561234269E-2</v>
-      </c>
-      <c r="T57">
-        <v>6.8890351745199002E-2</v>
-      </c>
-      <c r="U57">
-        <v>6.6864164929163736E-2</v>
-      </c>
-      <c r="V57">
-        <v>6.4837978113128469E-2</v>
-      </c>
-      <c r="W57">
-        <v>6.2811791297093203E-2</v>
-      </c>
-      <c r="X57">
-        <v>6.078560448105793E-2</v>
-      </c>
-      <c r="Y57">
-        <v>5.8759417665022663E-2</v>
-      </c>
-      <c r="Z57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AA57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AB57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AC57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AD57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AE57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AF57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AG57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AH57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AI57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AJ57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AK57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AL57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AM57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AN57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AO57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AP57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AQ57">
-        <v>5.6733230848987397E-2</v>
-      </c>
-      <c r="AR57">
-        <v>5.6733230848987397E-2</v>
       </c>
     </row>
     <row r="58" spans="1:44">
@@ -15693,7 +15500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">

</xml_diff>

<commit_message>
Finish fixes to test cases so CI/CD can work again.
Signed-off-by: MichaelTiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/test_data_company.xlsx
+++ b/test/inputs/test_data_company.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casj\PycharmProjects\ITR\test\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR-MichaelTiemannOSC/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAC0AB0-68AB-4808-AF5B-BD21E051D5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DBC667-5F09-E340-8F31-AA4E441FE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="69060" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,24 +768,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +841,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -858,10 +858,10 @@
         <v>91</v>
       </c>
       <c r="K2">
-        <v>104827858.636039</v>
+        <v>640885111.27013505</v>
       </c>
       <c r="L2">
-        <v>104827858.636039</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>20248547996.814301</v>
@@ -882,7 +882,7 @@
         <v>0.42857142857142799</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
@@ -899,10 +899,10 @@
         <v>91</v>
       </c>
       <c r="K3">
-        <v>598937001.89205897</v>
+        <v>1027603972.59417</v>
       </c>
       <c r="L3">
-        <v>598937001.89205897</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>276185899.61435097</v>
@@ -923,7 +923,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
@@ -940,10 +940,10 @@
         <v>91</v>
       </c>
       <c r="K4">
-        <v>122472002.66109601</v>
+        <v>1807821.3453092501</v>
       </c>
       <c r="L4">
-        <v>122472002.66109601</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>10283015131.798985</v>
@@ -964,7 +964,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>75</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>76</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>77</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>78</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>79</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>80</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>84</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>85</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>87</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>88</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>47</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>51</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>53</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
@@ -2047,79 +2047,79 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="16:16">
+    <row r="33" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="16:16">
+    <row r="34" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="16:16">
+    <row r="35" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="16:16">
+    <row r="36" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="16:16">
+    <row r="37" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="16:16">
+    <row r="38" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="16:16">
+    <row r="39" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="16:16">
+    <row r="40" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="16:16">
+    <row r="41" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="16:16">
+    <row r="42" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="16:16">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P43" s="2"/>
     </row>
-    <row r="44" spans="16:16">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="16:16">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="16:16">
+    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="16:16">
+    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="16:16">
+    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="16:16">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P49" s="2"/>
     </row>
-    <row r="50" spans="16:16">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="16:16">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P51" s="2"/>
     </row>
-    <row r="52" spans="16:16">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="16:16">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P53" s="2"/>
     </row>
-    <row r="54" spans="16:16">
+    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P54" s="2"/>
     </row>
-    <row r="55" spans="16:16">
+    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="16:16">
+    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P56" s="2"/>
     </row>
   </sheetData>
@@ -2136,19 +2136,19 @@
   <dimension ref="A1:P145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>49092005.8360392</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>359005.836039191</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>104827858.636039</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0.46831068071786103</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>3.4247178251122501E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>64776309.492059298</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>14514120.492059199</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>598937001.89205897</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>2.4233133779026399E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>141300001.396088</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>9500001.3960884009</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>71500001.396088406</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>8530004.4552317206</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>1750004.4552317201</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>25</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>27</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>20351815.8145184</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>1181783.8145184</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>3.1695179636323602E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>3.9975093970069597E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>33100009.401725199</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>290009.40172515198</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>100080009.40172499</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>0.33073547454277702</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>2.89777552439111E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>45260006.4724712</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>9</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>5000006.4724712502</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>9</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>745588806.472471</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>6.0703709711798497E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>9</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>6.7061179420427096E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>38589016.376334101</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>10</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>2330625.3763341298</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>10</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>199591200.37633401</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>10</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0.193340269027761</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>10</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>1.16769946367359E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>29</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>9056.9950820715403</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>29</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>2890986.4760820698</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>12194000.4760821</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>29</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>7.4274189998896497E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>29</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>0.23708269339111501</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>32</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>16442009.677026</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>32</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>5803009.6770260101</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>32</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>23303009.677026</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>0.70557451182951103</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>32</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>0.249024042707543</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>12</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>13136322.585938299</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>12</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>2001731.58593829</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>12</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>444466802.58593798</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>2.95552390178755E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>12</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>4.5036695075809496E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>35</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>52900000.2335485</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>35</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>7600000.2335484596</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>35</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>28090000.2335485</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>35</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>1.8832324597266801</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>35</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>0.27055892382911501</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>38</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>40045311.046821602</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>38</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>476901.04682159098</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>38</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>12630001.0468216</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>38</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>3.1706498596767099</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>38</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>3.7759383000336801E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>13</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>910000.85954060894</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>13</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>190000.859540609</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>13</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>1472652000.85954</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>13</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>6.1793340110866005E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>13</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>1.29019523573601E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>40</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>27206000.829291299</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>40</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>40</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>22329000.829291299</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>40</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>1.21841550534596</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>40</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>14</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>4500001.5077198902</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>14</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>2500001.5077198902</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>14</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>21142801.5077199</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>14</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>0.21283846921027899</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>14</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>0.118243625699606</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>42</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>84000001.367614105</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>42</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>9000001.3676141202</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>42</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>47050001.367614098</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>42</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>1.7853347274381499</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>42</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>0.191285889606989</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>44</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>28400004.631029598</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>44</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>3600004.6310295798</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>44</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>15520004.6310296</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>44</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>1.82989665958273</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>44</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>0.23195899206318399</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>16</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>226132940.90193</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>16</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>15845.901929563001</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>16</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>934632000.90192997</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>16</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>0.241948639340092</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>16</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>1.6954161546225199E-5</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>17</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>16065001.154934401</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>17</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>2403001.15493443</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>17</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>65804401.154934399</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>17</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>0.244132624459417</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>17</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>3.65173318616887E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>18</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>18</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>18</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>288420004.28137201</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>18</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>18</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>46</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>79447000.425667897</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>46</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>795000.42566793202</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>46</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>46</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>46</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>20</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>9681777.1404963192</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>20</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>1203273.1404963101</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>20</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>47691749.886496298</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>20</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>0.20300737891854301</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>20</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>2.52302157786208E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>21</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>70400001.129387006</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>21</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>2600001.1293870099</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>21</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>528390001.12938702</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>21</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>0.13323492302828099</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>21</v>
       </c>
@@ -8148,7 +8148,7 @@
         <v>4.9206100112222702E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>48</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>23400001.922484901</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>48</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>48</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>11314001.922484901</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>48</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>2.0682338647990499</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>48</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>52</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>9582000.0778485592</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>52</v>
       </c>
@@ -8498,7 +8498,7 @@
         <v>1173000.07784857</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>52</v>
       </c>
@@ -8548,7 +8548,7 @@
         <v>14473000.0778486</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>52</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>0.66206039012700302</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>52</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>8.1047472641410601E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>54</v>
       </c>
@@ -8698,7 +8698,7 @@
         <v>60116322</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>54</v>
       </c>
@@ -8748,7 +8748,7 @@
         <v>2779523</v>
       </c>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
         <v>54</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>28540004.3464472</v>
       </c>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>54</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>2.1063879763383277</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>54</v>
       </c>
@@ -8914,7 +8914,7 @@
         <v>9.7390419646029541E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>56</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>21300002.3736674</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>56</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>1400002.3736674299</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>56</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>56</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>56</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>22</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>48061950.558717303</v>
       </c>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>22</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>607645.55871729006</v>
       </c>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>22</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>242884801.55871701</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>22</v>
       </c>
@@ -9364,7 +9364,7 @@
         <v>0.19787961309344601</v>
       </c>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>22</v>
       </c>
@@ -9423,18 +9423,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="44" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -9568,7 +9568,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -9687,7 +9687,7 @@
         <v>8.911036813081348E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9806,7 +9806,7 @@
         <v>2.9611350252800795E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -9937,7 +9937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -10199,7 +10199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -10330,7 +10330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -10464,7 +10464,7 @@
         <v>5.3547663235850194E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -10598,7 +10598,7 @@
         <v>4.6916378754863521E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>1.7066206031018747E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -10860,7 +10860,7 @@
         <v>1.1222324393279194E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -10991,7 +10991,7 @@
         <v>5.0006792876853574E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -11122,7 +11122,7 @@
         <v>3.0202143358947035E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -11384,7 +11384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>1.8395932677230543E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -11634,7 +11634,7 @@
         <v>1.5253008327079058E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -11884,7 +11884,7 @@
         <v>8.5331905004060842E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -12015,7 +12015,7 @@
         <v>7.8258982440232314E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -12140,7 +12140,7 @@
         <v>7.6393565059035713E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -12271,7 +12271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:44">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -12402,7 +12402,7 @@
         <v>7.4930186515361902E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:44">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -12500,7 +12500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:44">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -12508,7 +12508,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:44">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -12642,7 +12642,7 @@
         <v>7.8691147818454946E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:44">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>1.9940079263305985E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:44">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -12904,7 +12904,7 @@
         <v>3.2513089908839096E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:44">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -13035,7 +13035,7 @@
         <v>1.2007680273680536E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:44">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -13169,7 +13169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:44">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -13303,7 +13303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:44">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:44">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -13541,7 +13541,7 @@
         <v>2.3531717117231055E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:44">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -13549,7 +13549,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:44">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -13557,7 +13557,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:44">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -13565,7 +13565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:44">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:44">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -13677,7 +13677,7 @@
         <v>5.3112528078259186E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:44">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -13781,7 +13781,7 @@
         <v>6.8687840496457889E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:44">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -13900,7 +13900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:44">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -14019,7 +14019,7 @@
         <v>6.5898648327123444E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:44">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:44">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -14245,7 +14245,7 @@
         <v>6.7336740335270401E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:44">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -14364,7 +14364,7 @@
         <v>2.1165034305152708</v>
       </c>
     </row>
-    <row r="45" spans="1:44">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -14483,7 +14483,7 @@
         <v>1.7283227911659416E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:44">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>1.0443561474393943</v>
       </c>
     </row>
-    <row r="47" spans="1:44">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -14529,7 +14529,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:44">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -14642,7 +14642,7 @@
         <v>1.1291898788025883</v>
       </c>
     </row>
-    <row r="49" spans="1:44">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -14755,7 +14755,7 @@
         <v>2.9126792689964681E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:44">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -14871,7 +14871,7 @@
         <v>1.1503609148905434</v>
       </c>
     </row>
-    <row r="51" spans="1:44">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -14987,7 +14987,7 @@
         <v>7.2197212871397132E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:44">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -14995,7 +14995,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:44">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -15003,7 +15003,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:44">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -15041,7 +15041,7 @@
         <v>1.7773884775616839</v>
       </c>
     </row>
-    <row r="55" spans="1:44">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -15049,7 +15049,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:44">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -15057,7 +15057,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:44">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -15065,7 +15065,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:44">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>1.5067587714222448</v>
       </c>
     </row>
-    <row r="59" spans="1:44">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -15303,7 +15303,7 @@
         <v>2.82160520232232E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:44">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -15398,7 +15398,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:44">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -15503,18 +15503,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46:M47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="44" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -15648,7 +15648,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -15767,7 +15767,7 @@
         <v>8.9465911484951893E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -15886,7 +15886,7 @@
         <v>2.9611350252800795E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -16017,7 +16017,7 @@
         <v>2.7093533847900943E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -16148,7 +16148,7 @@
         <v>4.2782297907073925E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -16279,7 +16279,7 @@
         <v>1.3123562059001663E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -16410,7 +16410,7 @@
         <v>2.6896752755997291E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -16544,7 +16544,7 @@
         <v>5.3969490446003025E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -16678,7 +16678,7 @@
         <v>4.7336577395813443E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -16809,7 +16809,7 @@
         <v>1.7829327732493332E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -16940,7 +16940,7 @@
         <v>1.1222324393279194E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -17071,7 +17071,7 @@
         <v>5.2654499665761639E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -17202,7 +17202,7 @@
         <v>3.7250754698664E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -17333,7 +17333,7 @@
         <v>6.5794162297210567E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -17464,7 +17464,7 @@
         <v>1.1695895122326271E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -17589,7 +17589,7 @@
         <v>1.8395932677230543E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -17714,7 +17714,7 @@
         <v>1.5253008327079058E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>6.7720483867934181E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -17964,7 +17964,7 @@
         <v>8.5331905004060842E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -18095,7 +18095,7 @@
         <v>7.8258982440232314E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -18220,7 +18220,7 @@
         <v>7.6393565059035713E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -18351,7 +18351,7 @@
         <v>7.6239353663867096E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:44">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -18482,7 +18482,7 @@
         <v>7.4930186515361902E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:44">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -18580,7 +18580,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:44">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -18675,7 +18675,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:44">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -18809,7 +18809,7 @@
         <v>7.8691147818454946E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:44">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -18940,7 +18940,7 @@
         <v>1.9940079263305985E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:44">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -19071,7 +19071,7 @@
         <v>3.3560366404392354E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:44">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -19202,7 +19202,7 @@
         <v>1.5349153181480155E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:44">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -19336,7 +19336,7 @@
         <v>5.5505013727301572E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:44">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -19470,7 +19470,7 @@
         <v>4.3891690190548177E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:44">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -19589,7 +19589,7 @@
         <v>1.4001181795063664</v>
       </c>
     </row>
-    <row r="33" spans="1:44">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -19708,7 +19708,7 @@
         <v>2.3531717117231055E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:44">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -19806,7 +19806,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:44">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -19901,7 +19901,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:44">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -19999,7 +19999,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:44">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -20094,7 +20094,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:44">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -20198,7 +20198,7 @@
         <v>5.3112528078259186E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:44">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -20302,7 +20302,7 @@
         <v>6.8687840496457889E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:44">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -20421,7 +20421,7 @@
         <v>0.57154725873015932</v>
       </c>
     </row>
-    <row r="41" spans="1:44">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -20540,7 +20540,7 @@
         <v>6.5898648327123444E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:44">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -20653,7 +20653,7 @@
         <v>1.2851667278216812</v>
       </c>
     </row>
-    <row r="43" spans="1:44">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -20766,7 +20766,7 @@
         <v>6.7336740335270401E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:44">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -20885,7 +20885,7 @@
         <v>2.1165034305152708</v>
       </c>
     </row>
-    <row r="45" spans="1:44">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -21004,7 +21004,7 @@
         <v>1.7283227911659416E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:44">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -21117,7 +21117,7 @@
         <v>0.56647178234635764</v>
       </c>
     </row>
-    <row r="47" spans="1:44">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -21212,7 +21212,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:44">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -21325,7 +21325,7 @@
         <v>1.1291898788025883</v>
       </c>
     </row>
-    <row r="49" spans="1:44">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -21438,7 +21438,7 @@
         <v>2.9126792689964681E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:44">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -21554,7 +21554,7 @@
         <v>1.2239842634861196</v>
       </c>
     </row>
-    <row r="51" spans="1:44">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -21670,7 +21670,7 @@
         <v>7.2197212871397132E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:44">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -21768,7 +21768,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:44">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -21863,7 +21863,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:44">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -21976,7 +21976,7 @@
         <v>2.5859784627862941</v>
       </c>
     </row>
-    <row r="55" spans="1:44">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -22071,7 +22071,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:44">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -22181,7 +22181,7 @@
         <v>0.51622338238895638</v>
       </c>
     </row>
-    <row r="57" spans="1:44">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -22291,7 +22291,7 @@
         <v>2.4817386351185876E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:44">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -22410,7 +22410,7 @@
         <v>1.5067587714222448</v>
       </c>
     </row>
-    <row r="59" spans="1:44">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -22529,12 +22529,12 @@
         <v>2.82160520232232E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:44">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:44">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Get excel.py working, fixing and harmonizing as we go...
Signed-off-by: MichaelTiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/test_data_company.xlsx
+++ b/test/inputs/test_data_company.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11009"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR-MichaelTiemannOSC/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DBC667-5F09-E340-8F31-AA4E441FE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D830C991-F504-2247-BCB3-4CF8D9AB9DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="69060" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="69060" windowHeight="16900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
     <t>Production</t>
   </si>
   <si>
-    <t>Emission Intensities</t>
+    <t>Emissions Intensities</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
WIP: Most test cases now passing in some form or another.
There's still a lot of verification work that needs to go back in,
but the scopes work is starting to settle.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/test_data_company.xlsx
+++ b/test/inputs/test_data_company.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR-MichaelTiemannOSC/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Dropbox/My Mac (MacBook-Pro.local)/Documents/GitHub/MichaelTiemannOSC/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D830C991-F504-2247-BCB3-4CF8D9AB9DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F677CF0-CF0E-B840-ACEF-AA403CA1C426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="69060" windowHeight="16900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="16900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="historic_data" sheetId="7" r:id="rId2"/>
     <sheet name="projected_target" sheetId="6" r:id="rId3"/>
-    <sheet name="projected_ei_in_Wh" sheetId="5" r:id="rId4"/>
+    <sheet name="projected_ei" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -437,15 +437,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,7 +765,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
@@ -842,7 +841,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
@@ -883,7 +882,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B3" t="s">
@@ -924,7 +923,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B4" t="s">
@@ -965,7 +964,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B5" t="s">
@@ -1006,7 +1005,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B6" t="s">
@@ -1047,7 +1046,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B7" t="s">
@@ -1088,7 +1087,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B8" t="s">
@@ -1129,7 +1128,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B9" t="s">
@@ -1170,7 +1169,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B10" t="s">
@@ -1211,7 +1210,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B11" t="s">
@@ -1252,7 +1251,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B12" t="s">
@@ -1293,7 +1292,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B13" t="s">
@@ -1334,7 +1333,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B14" t="s">
@@ -1375,7 +1374,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" t="s">
@@ -1457,7 +1456,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B17" t="s">
@@ -1498,7 +1497,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B18" t="s">
@@ -1533,7 +1532,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B19" t="s">
@@ -1568,7 +1567,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B20" t="s">
@@ -1609,7 +1608,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B21" t="s">
@@ -1650,7 +1649,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B22" t="s">
@@ -1691,7 +1690,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
@@ -1732,7 +1731,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B24" t="s">
@@ -1773,7 +1772,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B25" t="s">
@@ -1814,7 +1813,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B26" t="s">
@@ -1855,7 +1854,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B27" t="s">
@@ -1890,7 +1889,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B28" t="s">
@@ -1931,7 +1930,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B29" t="s">
@@ -1972,7 +1971,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B30" t="s">
@@ -2013,7 +2012,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B31" t="s">
@@ -2046,81 +2045,6 @@
       <c r="R31">
         <v>0.42857142857142849</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P39" s="2"/>
-    </row>
-    <row r="40" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P40" s="2"/>
-    </row>
-    <row r="41" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P41" s="2"/>
-    </row>
-    <row r="42" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P42" s="2"/>
-    </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P43" s="2"/>
-    </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P44" s="2"/>
-    </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P45" s="2"/>
-    </row>
-    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P46" s="2"/>
-    </row>
-    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P48" s="2"/>
-    </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P49" s="2"/>
-    </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P50" s="2"/>
-    </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P51" s="2"/>
-    </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P52" s="2"/>
-    </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P53" s="2"/>
-    </row>
-    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P54" s="2"/>
-    </row>
-    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P55" s="2"/>
-    </row>
-    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P56" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2135,7 +2059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
@@ -2149,57 +2073,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>2009</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>2010</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>2011</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>2012</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>2013</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>2014</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>2015</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>2016</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>2017</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>2018</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="2">
         <v>2019</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="2">
         <v>2020</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P1" s="2">
         <v>2021</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -2249,7 +2173,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -2299,7 +2223,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -2349,7 +2273,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -2399,7 +2323,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -2449,7 +2373,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -2499,7 +2423,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
@@ -2549,7 +2473,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
@@ -2599,7 +2523,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
@@ -2611,13 +2535,13 @@
       <c r="D10" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>2.5057186553478599E-9</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>2.5397615768446099E-9</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>2.5747422593009901E-9</v>
       </c>
       <c r="H10">
@@ -2649,7 +2573,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
@@ -2699,7 +2623,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B12" t="s">
@@ -2749,7 +2673,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
@@ -2799,7 +2723,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
@@ -2849,7 +2773,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B15" t="s">
@@ -2899,7 +2823,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
@@ -2949,7 +2873,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B17" t="s">
@@ -2999,7 +2923,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
@@ -3049,7 +2973,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
@@ -3099,7 +3023,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
@@ -3149,7 +3073,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
@@ -3199,7 +3123,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B22" t="s">
@@ -3249,7 +3173,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
@@ -3299,7 +3223,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
@@ -3349,7 +3273,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
@@ -3399,7 +3323,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
@@ -3449,7 +3373,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B27" t="s">
@@ -3499,7 +3423,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
@@ -3549,7 +3473,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B29" t="s">
@@ -3599,7 +3523,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
@@ -3614,13 +3538,13 @@
       <c r="E30">
         <v>2.9553960401974502E-4</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>3.5896831063912501E-5</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>3.19938969396695E-5</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>6.7633770492123101E-5</v>
       </c>
       <c r="I30">
@@ -3649,7 +3573,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
@@ -3699,7 +3623,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B32" t="s">
@@ -3749,7 +3673,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
@@ -3799,7 +3723,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B34" t="s">
@@ -3849,7 +3773,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B35" t="s">
@@ -3899,7 +3823,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B36" t="s">
@@ -3949,7 +3873,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B37" t="s">
@@ -3999,7 +3923,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B38" t="s">
@@ -4049,7 +3973,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
@@ -4099,7 +4023,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B40" t="s">
@@ -4149,7 +4073,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B41" t="s">
@@ -4199,7 +4123,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B42" t="s">
@@ -4249,7 +4173,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B43" t="s">
@@ -4299,7 +4223,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B44" t="s">
@@ -4349,7 +4273,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B45" t="s">
@@ -4399,7 +4323,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B46" t="s">
@@ -4449,7 +4373,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B47" t="s">
@@ -4499,7 +4423,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B48" t="s">
@@ -4549,7 +4473,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B49" t="s">
@@ -4599,7 +4523,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B50" t="s">
@@ -4649,7 +4573,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B51" t="s">
@@ -4699,7 +4623,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B52" t="s">
@@ -4749,7 +4673,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B53" t="s">
@@ -4799,7 +4723,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B54" t="s">
@@ -4849,7 +4773,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B55" t="s">
@@ -4899,7 +4823,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B56" t="s">
@@ -4949,7 +4873,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B57" t="s">
@@ -4999,7 +4923,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B58" t="s">
@@ -5049,7 +4973,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B59" t="s">
@@ -5099,7 +5023,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B60" t="s">
@@ -5149,7 +5073,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B61" t="s">
@@ -5199,7 +5123,7 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B62" t="s">
@@ -5249,7 +5173,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B63" t="s">
@@ -5299,7 +5223,7 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B64" t="s">
@@ -5349,7 +5273,7 @@
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B65" t="s">
@@ -5399,7 +5323,7 @@
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B66" t="s">
@@ -5449,7 +5373,7 @@
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B67" t="s">
@@ -5499,7 +5423,7 @@
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B68" t="s">
@@ -5549,7 +5473,7 @@
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B69" t="s">
@@ -5599,7 +5523,7 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B70" t="s">
@@ -5617,13 +5541,13 @@
       <c r="F70" t="s">
         <v>109</v>
       </c>
-      <c r="G70" s="4">
+      <c r="G70" s="3">
         <v>8.2350581881727896E-5</v>
       </c>
-      <c r="H70" s="4">
+      <c r="H70" s="3">
         <v>7.4186213652318599E-5</v>
       </c>
-      <c r="I70" s="4">
+      <c r="I70" s="3">
         <v>8.7802886405047395E-5</v>
       </c>
       <c r="J70">
@@ -5649,7 +5573,7 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B71" t="s">
@@ -5699,7 +5623,7 @@
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B72" t="s">
@@ -5749,7 +5673,7 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B73" t="s">
@@ -5799,7 +5723,7 @@
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B74" t="s">
@@ -5849,7 +5773,7 @@
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B75" t="s">
@@ -5899,7 +5823,7 @@
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B76" t="s">
@@ -5949,7 +5873,7 @@
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B77" t="s">
@@ -5999,7 +5923,7 @@
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B78" t="s">
@@ -6049,7 +5973,7 @@
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B79" t="s">
@@ -6099,7 +6023,7 @@
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B80" t="s">
@@ -6149,7 +6073,7 @@
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B81" t="s">
@@ -6199,7 +6123,7 @@
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B82" t="s">
@@ -6249,7 +6173,7 @@
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B83" t="s">
@@ -6299,7 +6223,7 @@
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B84" t="s">
@@ -6349,7 +6273,7 @@
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B85" t="s">
@@ -6399,7 +6323,7 @@
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B86" t="s">
@@ -6449,7 +6373,7 @@
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B87" t="s">
@@ -6499,7 +6423,7 @@
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B88" t="s">
@@ -6549,7 +6473,7 @@
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B89" t="s">
@@ -6599,7 +6523,7 @@
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B90" t="s">
@@ -6649,7 +6573,7 @@
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B91" t="s">
@@ -6699,7 +6623,7 @@
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B92" t="s">
@@ -6749,7 +6673,7 @@
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B93" t="s">
@@ -6799,7 +6723,7 @@
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B94" t="s">
@@ -6849,7 +6773,7 @@
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B95" t="s">
@@ -6867,39 +6791,39 @@
       <c r="F95" t="s">
         <v>109</v>
       </c>
-      <c r="G95" s="4">
+      <c r="G95" s="3">
         <v>1.1281847590104501E-9</v>
       </c>
-      <c r="H95" s="4">
+      <c r="H95" s="3">
         <v>1.07976618962186E-9</v>
       </c>
-      <c r="I95" s="4">
+      <c r="I95" s="3">
         <v>1.07395273335092E-9</v>
       </c>
-      <c r="J95" s="4">
+      <c r="J95" s="3">
         <v>7.1788094253873198E-6</v>
       </c>
-      <c r="K95" s="4">
+      <c r="K95" s="3">
         <v>1.43138630794245E-5</v>
       </c>
-      <c r="L95" s="4">
+      <c r="L95" s="3">
         <v>2.07557732976029E-5</v>
       </c>
-      <c r="M95" s="4">
+      <c r="M95" s="3">
         <v>2.6061274042782299E-5</v>
       </c>
-      <c r="N95" s="4">
+      <c r="N95" s="3">
         <v>2.3550537345723801E-5</v>
       </c>
-      <c r="O95" s="4">
+      <c r="O95" s="3">
         <v>1.6954161546225199E-5</v>
       </c>
-      <c r="P95" s="4">
+      <c r="P95" s="3">
         <v>1.6954161546225199E-5</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B96" t="s">
@@ -6949,7 +6873,7 @@
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B97" t="s">
@@ -6999,7 +6923,7 @@
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B98" t="s">
@@ -7049,7 +6973,7 @@
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B99" t="s">
@@ -7099,7 +7023,7 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B100" t="s">
@@ -7149,7 +7073,7 @@
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B101" t="s">
@@ -7199,7 +7123,7 @@
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B102" t="s">
@@ -7249,7 +7173,7 @@
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B103" t="s">
@@ -7299,7 +7223,7 @@
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B104" t="s">
@@ -7349,7 +7273,7 @@
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B105" t="s">
@@ -7399,7 +7323,7 @@
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B106" t="s">
@@ -7449,7 +7373,7 @@
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B107" t="s">
@@ -7499,7 +7423,7 @@
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B108" t="s">
@@ -7549,7 +7473,7 @@
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B109" t="s">
@@ -7599,7 +7523,7 @@
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B110" t="s">
@@ -7649,7 +7573,7 @@
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B111" t="s">
@@ -7699,7 +7623,7 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B112" t="s">
@@ -7749,7 +7673,7 @@
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B113" t="s">
@@ -7799,7 +7723,7 @@
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B114" t="s">
@@ -7849,7 +7773,7 @@
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B115" t="s">
@@ -7861,13 +7785,13 @@
       <c r="D115" t="s">
         <v>109</v>
       </c>
-      <c r="E115" s="4">
+      <c r="E115" s="3">
         <v>5.2427676449402701E-8</v>
       </c>
-      <c r="F115" s="4">
+      <c r="F115" s="3">
         <v>5.2622557615435301E-8</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G115" s="3">
         <v>5.3876610887202302E-8</v>
       </c>
       <c r="H115">
@@ -7899,7 +7823,7 @@
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B116" t="s">
@@ -7949,7 +7873,7 @@
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B117" t="s">
@@ -7999,7 +7923,7 @@
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B118" t="s">
@@ -8049,7 +7973,7 @@
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B119" t="s">
@@ -8099,7 +8023,7 @@
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B120" t="s">
@@ -8149,7 +8073,7 @@
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B121" t="s">
@@ -8199,7 +8123,7 @@
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B122" t="s">
@@ -8249,7 +8173,7 @@
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B123" t="s">
@@ -8299,7 +8223,7 @@
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B124" t="s">
@@ -8349,7 +8273,7 @@
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B125" t="s">
@@ -8399,7 +8323,7 @@
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B126" t="s">
@@ -8449,7 +8373,7 @@
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B127" t="s">
@@ -8499,7 +8423,7 @@
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B128" t="s">
@@ -8549,7 +8473,7 @@
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B129" t="s">
@@ -8599,7 +8523,7 @@
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B130" t="s">
@@ -8649,7 +8573,7 @@
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B131" t="s">
@@ -8699,7 +8623,7 @@
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A132" s="5" t="s">
+      <c r="A132" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B132" t="s">
@@ -8749,7 +8673,7 @@
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A133" s="5" t="s">
+      <c r="A133" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B133" t="s">
@@ -8799,7 +8723,7 @@
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B134" t="s">
@@ -8857,7 +8781,7 @@
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A135" s="5" t="s">
+      <c r="A135" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B135" t="s">
@@ -8915,7 +8839,7 @@
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A136" s="5" t="s">
+      <c r="A136" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B136" t="s">
@@ -8965,7 +8889,7 @@
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B137" t="s">
@@ -9015,7 +8939,7 @@
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A138" s="5" t="s">
+      <c r="A138" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B138" t="s">
@@ -9065,7 +8989,7 @@
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A139" s="5" t="s">
+      <c r="A139" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B139" t="s">
@@ -9115,7 +9039,7 @@
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A140" s="5" t="s">
+      <c r="A140" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B140" t="s">
@@ -9165,7 +9089,7 @@
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A141" s="5" t="s">
+      <c r="A141" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B141" t="s">
@@ -9215,7 +9139,7 @@
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A142" s="5" t="s">
+      <c r="A142" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B142" t="s">
@@ -9265,7 +9189,7 @@
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A143" s="5" t="s">
+      <c r="A143" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B143" t="s">
@@ -9315,7 +9239,7 @@
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A144" s="5" t="s">
+      <c r="A144" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B144" t="s">
@@ -9365,7 +9289,7 @@
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A145" s="5" t="s">
+      <c r="A145" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B145" t="s">
@@ -15503,7 +15427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>